<commit_message>
Update: Data dictionary and README
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MADS\SIADS 593 - Milestone I\online-learning-so-mooc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC26B948-F819-4FCE-A6E1-A30974ABCA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50741D43-370A-4983-B5FB-375233900548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="21690" xr2:uid="{37195A6E-FA30-4916-932A-59A154A1E688}"/>
+    <workbookView xWindow="13030" yWindow="1200" windowWidth="17680" windowHeight="18040" activeTab="1" xr2:uid="{37195A6E-FA30-4916-932A-59A154A1E688}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Combined MOOC" sheetId="1" r:id="rId1"/>
+    <sheet name="Stack Overflow Survey" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="128">
   <si>
     <t>Data Type</t>
   </si>
@@ -246,6 +247,246 @@
   </si>
   <si>
     <t>[5, 5, 5]</t>
+  </si>
+  <si>
+    <t>survey_results</t>
+  </si>
+  <si>
+    <t>CodingStatus</t>
+  </si>
+  <si>
+    <t>Describes the current coding status of the survey respondent.</t>
+  </si>
+  <si>
+    <t>I am a developer by profession 
+I am learning to code 
+I code primarily as a hobby 
+I am not primarily a developer, but I write code sometimes as part of my work/studies 
+I used to be a developer by profession, but no longer am</t>
+  </si>
+  <si>
+    <t>AgeRange</t>
+  </si>
+  <si>
+    <t>The age range of the survey respondent.</t>
+  </si>
+  <si>
+    <t>Under 18 years old
+18-24 years old
+25-34 years old
+35-44 years old
+45-54 years old
+55-64 years old
+65 years or older
+Prefer not to say</t>
+  </si>
+  <si>
+    <t>EducationLevel</t>
+  </si>
+  <si>
+    <t>The highest education level achieved by the survey respondent.</t>
+  </si>
+  <si>
+    <t>Primary/elementary school
+Secondary school (e.g. American high school, German Realschule or Gymnasium, etc.)
+Associate degree (A.A., A.S., etc.)
+Bachelor’s degree (B.A., B.S., B.Eng., etc.)
+Master’s degree (M.A., M.S., M.Eng., MBA, etc.)
+Professional degree (JD, MD, Ph.D, Ed.D, etc.)
+Some college/university study without earning a degree
+Something else</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>The country that the respondent is living in.</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>DevType</t>
+  </si>
+  <si>
+    <t>A description of the survey respondent's developer role.</t>
+  </si>
+  <si>
+    <t>Developer, full-stack
+Student
+Etc.</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>A description of the employment status of the survey respondent.</t>
+  </si>
+  <si>
+    <t>Employed, full-time
+Student, full-time
+Not employed, but looking for work
+Independent contractor, freelancer, or self-employed
+Not employed, and not looking for work
+Student, part-time
+Employed, part-time
+I prefer not to say
+Retired</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>A selection of the industry best matching the respondent's work industry.</t>
+  </si>
+  <si>
+    <t>Healthcare, Software Development, etc.</t>
+  </si>
+  <si>
+    <t>CodingActivities</t>
+  </si>
+  <si>
+    <t>A list of the different types of coding activities the respondent has participated in outside of work.</t>
+  </si>
+  <si>
+    <t>Hobby
+Contribute to open-source projects
+I don’t code outside of work
+Bootstrapping a business
+School or academic work
+Professional development or self-paced learning from online courses
+Freelance/contract work
+Other (please specify):</t>
+  </si>
+  <si>
+    <t>YearsCoding</t>
+  </si>
+  <si>
+    <t>The total number of years the respondent has spent coding including education, work experience, hobby coding, etc.</t>
+  </si>
+  <si>
+    <t>YearsCodingProfessional</t>
+  </si>
+  <si>
+    <t>Less than 1 year
+1...50
+More than 50 years</t>
+  </si>
+  <si>
+    <t>YearsWorkExperience</t>
+  </si>
+  <si>
+    <t>The total number of years of work experience the respondent has.</t>
+  </si>
+  <si>
+    <t>1...50</t>
+  </si>
+  <si>
+    <t>HowLearnCode</t>
+  </si>
+  <si>
+    <t>A list of the methods the respondent uses to learn coding skills.</t>
+  </si>
+  <si>
+    <t>Books / Physical media
+Colleague
+On the job training
+Other online resources (e.g., videos, blogs, forum, online community)
+School (i.e., University, College, etc)
+Online Courses or Certification
+Coding Bootcamp
+Friend or family member
+Other (please specify):</t>
+  </si>
+  <si>
+    <t>HowLearnCodeOnline</t>
+  </si>
+  <si>
+    <t>A list of the online resources the respondent uses to learn coding skills.</t>
+  </si>
+  <si>
+    <t>Technical documentation
+Blogs
+Books
+Etc.</t>
+  </si>
+  <si>
+    <t>LanguagesUsedPastYear</t>
+  </si>
+  <si>
+    <t>A list of all the programming languages the survey respondent has used in the past year.</t>
+  </si>
+  <si>
+    <t>HTML/CSS
+Java
+JavaScript
+Python
+Etc.</t>
+  </si>
+  <si>
+    <t>DatabasesUsedPastYear</t>
+  </si>
+  <si>
+    <t>A list of all the databases the survey respondent has used in the past year.</t>
+  </si>
+  <si>
+    <t>Dynamodb
+MongoDB
+PostgreSQL
+Etc.</t>
+  </si>
+  <si>
+    <t>PlatformsUsedPastYear</t>
+  </si>
+  <si>
+    <t>A list of all the cloud platforms the survey respondent has used in the past year.</t>
+  </si>
+  <si>
+    <t>Amazon Web Services (AWS)
+Heroku
+Netlify
+Etc.</t>
+  </si>
+  <si>
+    <t>WebFramworksUsedPastYear</t>
+  </si>
+  <si>
+    <t>A list of all the web frameworks the survey respondent has used in the past year.</t>
+  </si>
+  <si>
+    <t>Express
+Next.js
+Node.js
+Etc.</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>An indicator of the currency for the respondent's provided compensation number.</t>
+  </si>
+  <si>
+    <t>USD United States dollar
+BRL Brazilian real
+GBP Pound sterling
+RON Romanian leu
+Etc.</t>
+  </si>
+  <si>
+    <t>CompTotal</t>
+  </si>
+  <si>
+    <t>The respondents current total salary in the respondent's provided currency.</t>
+  </si>
+  <si>
+    <t>ConvertedCompYearly</t>
+  </si>
+  <si>
+    <t>The respondents total compensation converted to USD.
+THIS MUST BE VERIFIED DURING EDA - STACK OVERFLOW DOES NOT DOCUMENT THIS</t>
+  </si>
+  <si>
+    <t>Details from the Stack Overflow Developer Survey in 2024</t>
   </si>
 </sst>
 </file>
@@ -253,9 +494,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +519,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -312,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -335,11 +583,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -352,9 +630,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EF967D-751E-484A-AAD1-B537A2FDDA28}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,7 +1069,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
@@ -923,7 +1227,7 @@
       <c r="F12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>16</v>
       </c>
     </row>
@@ -963,7 +1267,7 @@
       <c r="F14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>1838</v>
       </c>
     </row>
@@ -1083,7 +1387,7 @@
       <c r="F20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1103,7 +1407,7 @@
       <c r="F21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1126,9 +1430,580 @@
       <c r="H22" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="8">
         <v>1</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671BAD1E-316B-4EE9-8246-4ECE41C4F28B}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="38.90625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="28.26953125" customWidth="1"/>
+    <col min="8" max="8" width="28.453125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="29.54296875" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="13">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="13">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="13">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="13">
+        <v>8</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="13">
+        <v>11</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="13">
+        <v>12</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="13">
+        <v>13</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="13">
+        <v>14</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="13">
+        <v>15</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="13">
+        <v>16</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="13">
+        <v>17</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="13">
+        <v>18</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="13">
+        <v>19</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="13">
+        <v>60000</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="13">
+        <v>20</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13">
+        <v>95000</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>